<commit_message>
lista 6, zaczecie wykresow, problem z quicksort, nie laduje sie na macu do .txt
</commit_message>
<xml_diff>
--- a/AiSD_Lab_Lista5/aisd_wykresy.xlsx
+++ b/AiSD_Lab_Lista5/aisd_wykresy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Documents/Development/AiSD_Lab/AiSD_Lab_Lista5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19FA09A-907C-CC4E-852B-882C61B8DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4128C9A1-5CC2-3D4D-B3FF-2A0C40C2DE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20140" activeTab="2" xr2:uid="{C7128112-AAFE-497F-80CF-4D7C130D65FB}"/>
+    <workbookView xWindow="0" yWindow="3860" windowWidth="29400" windowHeight="17140" activeTab="2" xr2:uid="{C7128112-AAFE-497F-80CF-4D7C130D65FB}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderedGenerator" sheetId="1" r:id="rId1"/>

</xml_diff>